<commit_message>
applied multi threading application in the JournalApp and colored chart by recived output
</commit_message>
<xml_diff>
--- a/trading_journal.xlsx
+++ b/trading_journal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Cloud Files\TradingTools\trade_journal_project\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Cloud Files\TradingTools\trade_journal_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7986EA2F-BD4B-4516-A1DB-0CFFDBA9C7BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E58C2E-A040-479A-9EED-0E47942485D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="67">
   <si>
     <t>Sector</t>
   </si>
@@ -232,13 +232,19 @@
   </si>
   <si>
     <t>Entry Label</t>
+  </si>
+  <si>
+    <t>mkt</t>
+  </si>
+  <si>
+    <t>lmt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,8 +327,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="27">
+  <fills count="32">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -472,6 +486,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFBE7D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1074,7 +1118,7 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1189,9 +1233,6 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="28" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1199,9 +1240,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1231,15 +1269,9 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1261,6 +1293,51 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="35" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1291,50 +1368,14 @@
     <xf numFmtId="0" fontId="5" fillId="24" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="15" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="16" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1348,14 +1389,26 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="15" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="16" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="17" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="18" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="19" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1366,27 +1419,6 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="17" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="18" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="19" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1404,6 +1436,39 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="16" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1422,6 +1487,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFD961"/>
       <color rgb="FFFFBE7D"/>
       <color rgb="FF79CDB5"/>
       <color rgb="FF4784FF"/>
@@ -1430,7 +1496,6 @@
       <color rgb="FF6598FF"/>
       <color rgb="FFE79D5F"/>
       <color rgb="FFFFCD2F"/>
-      <color rgb="FFFFD961"/>
       <color rgb="FFFFCB25"/>
     </mruColors>
   </colors>
@@ -1711,37 +1776,37 @@
   <dimension ref="A1:BC26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="U19" sqref="U19"/>
+      <selection pane="bottomRight" activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" thickBottom="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" style="50" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" style="53" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.109375" style="51" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="10.6640625" style="51" customWidth="1"/>
-    <col min="11" max="12" width="12.6640625" style="51" customWidth="1"/>
-    <col min="13" max="13" width="15.109375" style="51" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="12.6640625" style="51" customWidth="1"/>
-    <col min="18" max="18" width="22.5546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="19" max="24" width="10.6640625" style="51" customWidth="1"/>
-    <col min="25" max="25" width="17.33203125" style="51" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.88671875" style="51" bestFit="1" customWidth="1"/>
-    <col min="27" max="30" width="10.6640625" style="51" customWidth="1"/>
-    <col min="31" max="31" width="24.33203125" style="51" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="24.33203125" style="51" customWidth="1"/>
-    <col min="33" max="33" width="13.44140625" style="51" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="22.5546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="30.6640625" style="51" customWidth="1"/>
-    <col min="36" max="36" width="22.5546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="19.109375" style="63" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="19.109375" style="65" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" style="49" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" style="51" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" style="50" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" style="50" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="10.6640625" style="50" customWidth="1"/>
+    <col min="11" max="12" width="12.6640625" style="50" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" style="50" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="12.6640625" style="50" customWidth="1"/>
+    <col min="18" max="18" width="22.5546875" style="50" bestFit="1" customWidth="1"/>
+    <col min="19" max="24" width="10.6640625" style="50" customWidth="1"/>
+    <col min="25" max="25" width="17.33203125" style="50" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.88671875" style="50" bestFit="1" customWidth="1"/>
+    <col min="27" max="30" width="10.6640625" style="50" customWidth="1"/>
+    <col min="31" max="31" width="24.33203125" style="50" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="24.33203125" style="50" customWidth="1"/>
+    <col min="33" max="33" width="13.44140625" style="50" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="22.5546875" style="50" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="30.6640625" style="50" customWidth="1"/>
+    <col min="36" max="36" width="22.5546875" style="50" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="19.109375" style="60" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="19.109375" style="61" bestFit="1" customWidth="1"/>
     <col min="39" max="45" width="8.88671875" style="5"/>
     <col min="46" max="55" width="8.88671875" style="6"/>
     <col min="56" max="16384" width="8.88671875" style="1"/>
@@ -1750,44 +1815,44 @@
     <row r="1" spans="1:55" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
-      <c r="C1" s="82" t="s">
+      <c r="C1" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="82"/>
-      <c r="U1" s="82"/>
-      <c r="V1" s="82"/>
-      <c r="W1" s="82"/>
-      <c r="X1" s="82"/>
-      <c r="Y1" s="82"/>
-      <c r="Z1" s="82"/>
-      <c r="AA1" s="82"/>
-      <c r="AB1" s="82"/>
-      <c r="AC1" s="82"/>
-      <c r="AD1" s="82"/>
-      <c r="AE1" s="82"/>
-      <c r="AF1" s="82"/>
-      <c r="AG1" s="82"/>
-      <c r="AH1" s="82"/>
-      <c r="AI1" s="82"/>
-      <c r="AJ1" s="82"/>
-      <c r="AK1" s="82"/>
-      <c r="AL1" s="82"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="68"/>
+      <c r="S1" s="68"/>
+      <c r="T1" s="68"/>
+      <c r="U1" s="68"/>
+      <c r="V1" s="68"/>
+      <c r="W1" s="68"/>
+      <c r="X1" s="68"/>
+      <c r="Y1" s="68"/>
+      <c r="Z1" s="68"/>
+      <c r="AA1" s="68"/>
+      <c r="AB1" s="68"/>
+      <c r="AC1" s="68"/>
+      <c r="AD1" s="68"/>
+      <c r="AE1" s="68"/>
+      <c r="AF1" s="68"/>
+      <c r="AG1" s="68"/>
+      <c r="AH1" s="68"/>
+      <c r="AI1" s="68"/>
+      <c r="AJ1" s="68"/>
+      <c r="AK1" s="68"/>
+      <c r="AL1" s="68"/>
       <c r="AM1" s="4"/>
       <c r="AN1" s="4"/>
       <c r="AO1" s="4"/>
@@ -1851,143 +1916,143 @@
       <c r="BC2" s="7"/>
     </row>
     <row r="3" spans="1:55" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="93" t="s">
+      <c r="C3" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="85" t="s">
+      <c r="D3" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="95" t="s">
+      <c r="E3" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="95" t="s">
+      <c r="F3" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="92" t="s">
+      <c r="G3" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92" t="s">
+      <c r="H3" s="78"/>
+      <c r="I3" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="92"/>
-      <c r="K3" s="78" t="s">
+      <c r="J3" s="78"/>
+      <c r="K3" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="79"/>
-      <c r="M3" s="79"/>
-      <c r="N3" s="79"/>
-      <c r="O3" s="79"/>
-      <c r="P3" s="79"/>
-      <c r="Q3" s="80"/>
-      <c r="R3" s="89" t="s">
+      <c r="L3" s="90"/>
+      <c r="M3" s="90"/>
+      <c r="N3" s="90"/>
+      <c r="O3" s="90"/>
+      <c r="P3" s="90"/>
+      <c r="Q3" s="91"/>
+      <c r="R3" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="89"/>
-      <c r="T3" s="89"/>
-      <c r="U3" s="89"/>
-      <c r="V3" s="81" t="s">
+      <c r="S3" s="75"/>
+      <c r="T3" s="75"/>
+      <c r="U3" s="75"/>
+      <c r="V3" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="W3" s="81"/>
-      <c r="X3" s="81"/>
-      <c r="Y3" s="87" t="s">
+      <c r="W3" s="92"/>
+      <c r="X3" s="92"/>
+      <c r="Y3" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="Z3" s="87" t="s">
+      <c r="Z3" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="AA3" s="75" t="s">
+      <c r="AA3" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="AB3" s="75"/>
-      <c r="AC3" s="72" t="s">
+      <c r="AB3" s="86"/>
+      <c r="AC3" s="83" t="s">
         <v>16</v>
       </c>
-      <c r="AD3" s="73"/>
-      <c r="AE3" s="73"/>
-      <c r="AF3" s="73"/>
-      <c r="AG3" s="73"/>
-      <c r="AH3" s="74"/>
-      <c r="AI3" s="76" t="s">
+      <c r="AD3" s="84"/>
+      <c r="AE3" s="84"/>
+      <c r="AF3" s="84"/>
+      <c r="AG3" s="84"/>
+      <c r="AH3" s="85"/>
+      <c r="AI3" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="AJ3" s="76" t="s">
+      <c r="AJ3" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="AK3" s="83" t="s">
+      <c r="AK3" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="AL3" s="90" t="s">
+      <c r="AL3" s="76" t="s">
         <v>19</v>
       </c>
       <c r="AP3" s="6"/>
     </row>
     <row r="4" spans="1:55" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="94"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="67" t="s">
+      <c r="C4" s="80"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="67" t="s">
+      <c r="H4" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="67" t="s">
+      <c r="I4" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="67" t="s">
+      <c r="J4" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="68" t="s">
+      <c r="K4" s="64" t="s">
         <v>55</v>
       </c>
-      <c r="L4" s="68" t="s">
+      <c r="L4" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="M4" s="68" t="s">
+      <c r="M4" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="N4" s="68" t="s">
+      <c r="N4" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="68" t="s">
+      <c r="O4" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="68" t="s">
+      <c r="P4" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="68" t="s">
+      <c r="Q4" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="R4" s="69" t="s">
+      <c r="R4" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="S4" s="69" t="s">
+      <c r="S4" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="T4" s="69" t="s">
+      <c r="T4" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="U4" s="69" t="s">
+      <c r="U4" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="V4" s="70" t="s">
+      <c r="V4" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="W4" s="70" t="s">
+      <c r="W4" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="70" t="s">
+      <c r="X4" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="Y4" s="88"/>
-      <c r="Z4" s="88"/>
-      <c r="AA4" s="66" t="s">
+      <c r="Y4" s="74"/>
+      <c r="Z4" s="74"/>
+      <c r="AA4" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="AB4" s="66" t="s">
+      <c r="AB4" s="62" t="s">
         <v>5</v>
       </c>
       <c r="AC4" s="47" t="s">
@@ -2008,55 +2073,64 @@
       <c r="AH4" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="AI4" s="77"/>
-      <c r="AJ4" s="77"/>
-      <c r="AK4" s="84"/>
-      <c r="AL4" s="91"/>
+      <c r="AI4" s="88"/>
+      <c r="AJ4" s="88"/>
+      <c r="AK4" s="70"/>
+      <c r="AL4" s="77"/>
     </row>
     <row r="5" spans="1:55" ht="14.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="48"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="49"/>
-      <c r="O5" s="49"/>
-      <c r="P5" s="49"/>
-      <c r="Q5" s="49"/>
-      <c r="R5" s="49"/>
-      <c r="S5" s="49"/>
-      <c r="T5" s="49"/>
-      <c r="U5" s="49"/>
-      <c r="V5" s="49"/>
-      <c r="W5" s="49"/>
-      <c r="X5" s="49"/>
-      <c r="Y5" s="49"/>
-      <c r="Z5" s="49"/>
-      <c r="AA5" s="49"/>
-      <c r="AB5" s="49"/>
-      <c r="AC5" s="49"/>
-      <c r="AD5" s="49"/>
-      <c r="AE5" s="49"/>
-      <c r="AF5" s="49"/>
-      <c r="AG5" s="49"/>
-      <c r="AH5" s="49"/>
-      <c r="AI5" s="49"/>
-      <c r="AJ5" s="49"/>
-      <c r="AK5" s="62"/>
-      <c r="AL5" s="64"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="116"/>
+      <c r="E5" s="119"/>
+      <c r="F5" s="117"/>
+      <c r="G5" s="120"/>
+      <c r="H5" s="120"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="117"/>
+      <c r="L5" s="117"/>
+      <c r="M5" s="120"/>
+      <c r="N5" s="117" t="s">
+        <v>66</v>
+      </c>
+      <c r="O5" s="117"/>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="48"/>
+      <c r="S5" s="48"/>
+      <c r="T5" s="48"/>
+      <c r="U5" s="48"/>
+      <c r="V5" s="117"/>
+      <c r="W5" s="120"/>
+      <c r="X5" s="120"/>
+      <c r="Y5" s="48"/>
+      <c r="Z5" s="122"/>
+      <c r="AA5" s="48"/>
+      <c r="AB5" s="48"/>
+      <c r="AC5" s="48"/>
+      <c r="AD5" s="48"/>
+      <c r="AE5" s="48"/>
+      <c r="AF5" s="48"/>
+      <c r="AG5" s="48"/>
+      <c r="AH5" s="48"/>
+      <c r="AI5" s="123"/>
+      <c r="AJ5" s="124"/>
+      <c r="AK5" s="125"/>
+      <c r="AL5" s="126"/>
+    </row>
+    <row r="6" spans="1:55" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N6" s="121" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="26" spans="34:35" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="AH26" s="53"/>
-      <c r="AI26" s="71"/>
+      <c r="AH26" s="51"/>
+      <c r="AI26" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="AI3:AI4"/>
     <mergeCell ref="C1:AL1"/>
     <mergeCell ref="AK3:AK4"/>
     <mergeCell ref="D3:D4"/>
@@ -2073,8 +2147,6 @@
     <mergeCell ref="AA3:AB3"/>
     <mergeCell ref="AJ3:AJ4"/>
     <mergeCell ref="K3:Q3"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="AI3:AI4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2111,64 +2183,64 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
       <c r="H2" s="23"/>
-      <c r="I2" s="107" t="s">
+      <c r="I2" s="100" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
-      <c r="L2" s="107"/>
-      <c r="M2" s="107"/>
-      <c r="N2" s="107"/>
-      <c r="O2" s="107"/>
-      <c r="P2" s="107"/>
-      <c r="Q2" s="107"/>
-      <c r="R2" s="107"/>
-      <c r="S2" s="107"/>
-      <c r="T2" s="107"/>
-      <c r="U2" s="107"/>
-      <c r="V2" s="107"/>
-      <c r="W2" s="107"/>
-      <c r="X2" s="107"/>
-      <c r="Y2" s="107"/>
-      <c r="Z2" s="107"/>
-      <c r="AA2" s="107"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
+      <c r="M2" s="100"/>
+      <c r="N2" s="100"/>
+      <c r="O2" s="100"/>
+      <c r="P2" s="100"/>
+      <c r="Q2" s="100"/>
+      <c r="R2" s="100"/>
+      <c r="S2" s="100"/>
+      <c r="T2" s="100"/>
+      <c r="U2" s="100"/>
+      <c r="V2" s="100"/>
+      <c r="W2" s="100"/>
+      <c r="X2" s="100"/>
+      <c r="Y2" s="100"/>
+      <c r="Z2" s="100"/>
+      <c r="AA2" s="100"/>
     </row>
     <row r="3" spans="1:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="107"/>
-      <c r="C3" s="107"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
       <c r="H3" s="23"/>
-      <c r="I3" s="107"/>
-      <c r="J3" s="107"/>
-      <c r="K3" s="107"/>
-      <c r="L3" s="107"/>
-      <c r="M3" s="107"/>
-      <c r="N3" s="107"/>
-      <c r="O3" s="107"/>
-      <c r="P3" s="107"/>
-      <c r="Q3" s="107"/>
-      <c r="R3" s="107"/>
-      <c r="S3" s="107"/>
-      <c r="T3" s="107"/>
-      <c r="U3" s="107"/>
-      <c r="V3" s="107"/>
-      <c r="W3" s="107"/>
-      <c r="X3" s="107"/>
-      <c r="Y3" s="107"/>
-      <c r="Z3" s="107"/>
-      <c r="AA3" s="107"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
+      <c r="P3" s="100"/>
+      <c r="Q3" s="100"/>
+      <c r="R3" s="100"/>
+      <c r="S3" s="100"/>
+      <c r="T3" s="100"/>
+      <c r="U3" s="100"/>
+      <c r="V3" s="100"/>
+      <c r="W3" s="100"/>
+      <c r="X3" s="100"/>
+      <c r="Y3" s="100"/>
+      <c r="Z3" s="100"/>
+      <c r="AA3" s="100"/>
     </row>
     <row r="4" spans="1:27" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="10"/>
@@ -2205,50 +2277,50 @@
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
-      <c r="J5" s="111" t="s">
+      <c r="J5" s="104" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="112"/>
-      <c r="L5" s="113"/>
+      <c r="K5" s="105"/>
+      <c r="L5" s="106"/>
       <c r="M5" s="14"/>
       <c r="N5" s="12"/>
-      <c r="O5" s="54" t="s">
+      <c r="O5" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="P5" s="55" t="s">
+      <c r="P5" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="Q5" s="56" t="s">
+      <c r="Q5" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="R5" s="57" t="s">
+      <c r="R5" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="S5" s="56" t="s">
+      <c r="S5" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="T5" s="57" t="s">
+      <c r="T5" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="U5" s="56" t="s">
+      <c r="U5" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="V5" s="57" t="s">
+      <c r="V5" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="W5" s="56" t="s">
+      <c r="W5" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="X5" s="57" t="s">
+      <c r="X5" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="Y5" s="56" t="s">
+      <c r="Y5" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="Z5" s="57" t="s">
+      <c r="Z5" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="AA5" s="58" t="s">
+      <c r="AA5" s="56" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2281,21 +2353,21 @@
       <c r="AA6" s="20"/>
     </row>
     <row r="7" spans="1:27" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="97" t="s">
+      <c r="B7" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="98"/>
-      <c r="D7" s="98"/>
-      <c r="E7" s="99"/>
-      <c r="F7" s="100"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="98"/>
+      <c r="F7" s="99"/>
       <c r="G7" s="24"/>
       <c r="I7" s="10"/>
-      <c r="J7" s="108" t="s">
+      <c r="J7" s="101" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="109"/>
-      <c r="L7" s="109"/>
-      <c r="M7" s="110"/>
+      <c r="K7" s="102"/>
+      <c r="L7" s="102"/>
+      <c r="M7" s="103"/>
       <c r="N7" s="15"/>
       <c r="O7" s="27"/>
       <c r="P7" s="28"/>
@@ -2312,21 +2384,21 @@
       <c r="AA7" s="32"/>
     </row>
     <row r="8" spans="1:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="104" t="s">
+      <c r="B8" s="107" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="105"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="106"/>
-      <c r="F8" s="100"/>
+      <c r="C8" s="108"/>
+      <c r="D8" s="108"/>
+      <c r="E8" s="109"/>
+      <c r="F8" s="99"/>
       <c r="G8" s="25"/>
       <c r="I8" s="10"/>
-      <c r="J8" s="59" t="s">
+      <c r="J8" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="61"/>
+      <c r="K8" s="58"/>
+      <c r="L8" s="58"/>
+      <c r="M8" s="59"/>
       <c r="N8" s="16"/>
       <c r="O8" s="33"/>
       <c r="P8" s="34"/>
@@ -2343,21 +2415,21 @@
       <c r="AA8" s="38"/>
     </row>
     <row r="9" spans="1:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="104" t="s">
+      <c r="B9" s="107" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="105"/>
-      <c r="D9" s="105"/>
-      <c r="E9" s="106"/>
-      <c r="F9" s="100"/>
+      <c r="C9" s="108"/>
+      <c r="D9" s="108"/>
+      <c r="E9" s="109"/>
+      <c r="F9" s="99"/>
       <c r="G9" s="25"/>
       <c r="I9" s="10"/>
-      <c r="J9" s="59" t="s">
+      <c r="J9" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="60"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="61"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="59"/>
       <c r="N9" s="17"/>
       <c r="O9" s="33"/>
       <c r="P9" s="34"/>
@@ -2374,21 +2446,21 @@
       <c r="AA9" s="38"/>
     </row>
     <row r="10" spans="1:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="104" t="s">
+      <c r="B10" s="107" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="105"/>
-      <c r="D10" s="105"/>
-      <c r="E10" s="106"/>
-      <c r="F10" s="100"/>
+      <c r="C10" s="108"/>
+      <c r="D10" s="108"/>
+      <c r="E10" s="109"/>
+      <c r="F10" s="99"/>
       <c r="G10" s="25"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="114" t="s">
+      <c r="J10" s="110" t="s">
         <v>28</v>
       </c>
-      <c r="K10" s="115"/>
-      <c r="L10" s="115"/>
-      <c r="M10" s="116"/>
+      <c r="K10" s="111"/>
+      <c r="L10" s="111"/>
+      <c r="M10" s="112"/>
       <c r="N10" s="17"/>
       <c r="O10" s="33"/>
       <c r="P10" s="34"/>
@@ -2405,21 +2477,21 @@
       <c r="AA10" s="38"/>
     </row>
     <row r="11" spans="1:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="101" t="s">
+      <c r="B11" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="102"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="103"/>
-      <c r="F11" s="100"/>
+      <c r="C11" s="94"/>
+      <c r="D11" s="94"/>
+      <c r="E11" s="95"/>
+      <c r="F11" s="99"/>
       <c r="G11" s="26"/>
       <c r="I11" s="10"/>
-      <c r="J11" s="117" t="s">
+      <c r="J11" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="K11" s="118"/>
-      <c r="L11" s="118"/>
-      <c r="M11" s="119"/>
+      <c r="K11" s="114"/>
+      <c r="L11" s="114"/>
+      <c r="M11" s="115"/>
       <c r="N11" s="21"/>
       <c r="O11" s="39"/>
       <c r="P11" s="40"/>
@@ -2465,22 +2537,22 @@
     </row>
     <row r="13" spans="1:27" s="7" customFormat="1" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
-      <c r="B13" s="97" t="s">
+      <c r="B13" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="98"/>
-      <c r="D13" s="98"/>
-      <c r="E13" s="99"/>
-      <c r="F13" s="100"/>
+      <c r="C13" s="97"/>
+      <c r="D13" s="97"/>
+      <c r="E13" s="98"/>
+      <c r="F13" s="99"/>
       <c r="G13" s="24"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
-      <c r="J13" s="97" t="s">
+      <c r="J13" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="K13" s="98"/>
-      <c r="L13" s="98"/>
-      <c r="M13" s="99"/>
+      <c r="K13" s="97"/>
+      <c r="L13" s="97"/>
+      <c r="M13" s="98"/>
       <c r="N13" s="22"/>
       <c r="O13" s="27"/>
       <c r="P13" s="28"/>
@@ -2498,22 +2570,22 @@
     </row>
     <row r="14" spans="1:27" s="7" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
-      <c r="B14" s="104" t="s">
+      <c r="B14" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="105"/>
-      <c r="D14" s="105"/>
-      <c r="E14" s="106"/>
-      <c r="F14" s="100"/>
+      <c r="C14" s="108"/>
+      <c r="D14" s="108"/>
+      <c r="E14" s="109"/>
+      <c r="F14" s="99"/>
       <c r="G14" s="25"/>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
-      <c r="J14" s="104" t="s">
+      <c r="J14" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="K14" s="105"/>
-      <c r="L14" s="105"/>
-      <c r="M14" s="106"/>
+      <c r="K14" s="108"/>
+      <c r="L14" s="108"/>
+      <c r="M14" s="109"/>
       <c r="N14" s="22"/>
       <c r="O14" s="33"/>
       <c r="P14" s="34"/>
@@ -2531,22 +2603,22 @@
     </row>
     <row r="15" spans="1:27" s="7" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
-      <c r="B15" s="101" t="s">
+      <c r="B15" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="102"/>
-      <c r="D15" s="102"/>
-      <c r="E15" s="103"/>
-      <c r="F15" s="100"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="95"/>
+      <c r="F15" s="99"/>
       <c r="G15" s="26"/>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
-      <c r="J15" s="101" t="s">
+      <c r="J15" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="K15" s="102"/>
-      <c r="L15" s="102"/>
-      <c r="M15" s="103"/>
+      <c r="K15" s="94"/>
+      <c r="L15" s="94"/>
+      <c r="M15" s="95"/>
       <c r="N15" s="22"/>
       <c r="O15" s="39"/>
       <c r="P15" s="40"/>
@@ -2591,22 +2663,22 @@
       <c r="AA16" s="46"/>
     </row>
     <row r="17" spans="2:27" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="97" t="s">
+      <c r="B17" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="98"/>
-      <c r="D17" s="98"/>
-      <c r="E17" s="99"/>
-      <c r="F17" s="100"/>
+      <c r="C17" s="97"/>
+      <c r="D17" s="97"/>
+      <c r="E17" s="98"/>
+      <c r="F17" s="99"/>
       <c r="G17" s="24"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="97" t="s">
+      <c r="J17" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="K17" s="98"/>
-      <c r="L17" s="98"/>
-      <c r="M17" s="99"/>
+      <c r="K17" s="97"/>
+      <c r="L17" s="97"/>
+      <c r="M17" s="98"/>
       <c r="N17" s="15"/>
       <c r="O17" s="27"/>
       <c r="P17" s="28"/>
@@ -2623,22 +2695,22 @@
       <c r="AA17" s="32"/>
     </row>
     <row r="18" spans="2:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="101" t="s">
+      <c r="B18" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="102"/>
-      <c r="D18" s="102"/>
-      <c r="E18" s="103"/>
-      <c r="F18" s="100"/>
+      <c r="C18" s="94"/>
+      <c r="D18" s="94"/>
+      <c r="E18" s="95"/>
+      <c r="F18" s="99"/>
       <c r="G18" s="26"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
-      <c r="J18" s="101" t="s">
+      <c r="J18" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="K18" s="102"/>
-      <c r="L18" s="102"/>
-      <c r="M18" s="103"/>
+      <c r="K18" s="94"/>
+      <c r="L18" s="94"/>
+      <c r="M18" s="95"/>
       <c r="N18" s="17"/>
       <c r="O18" s="39"/>
       <c r="P18" s="40"/>
@@ -2683,22 +2755,22 @@
       <c r="AA19" s="46"/>
     </row>
     <row r="20" spans="2:27" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="97" t="s">
+      <c r="B20" s="96" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="98"/>
-      <c r="D20" s="98"/>
-      <c r="E20" s="99"/>
-      <c r="F20" s="100"/>
+      <c r="C20" s="97"/>
+      <c r="D20" s="97"/>
+      <c r="E20" s="98"/>
+      <c r="F20" s="99"/>
       <c r="G20" s="24"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
-      <c r="J20" s="97" t="s">
+      <c r="J20" s="96" t="s">
         <v>52</v>
       </c>
-      <c r="K20" s="98"/>
-      <c r="L20" s="98"/>
-      <c r="M20" s="99"/>
+      <c r="K20" s="97"/>
+      <c r="L20" s="97"/>
+      <c r="M20" s="98"/>
       <c r="N20" s="15"/>
       <c r="O20" s="27"/>
       <c r="P20" s="28"/>
@@ -2715,22 +2787,22 @@
       <c r="AA20" s="32"/>
     </row>
     <row r="21" spans="2:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="101" t="s">
+      <c r="B21" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="102"/>
-      <c r="D21" s="102"/>
-      <c r="E21" s="103"/>
-      <c r="F21" s="100"/>
+      <c r="C21" s="94"/>
+      <c r="D21" s="94"/>
+      <c r="E21" s="95"/>
+      <c r="F21" s="99"/>
       <c r="G21" s="26"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="101" t="s">
+      <c r="J21" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="K21" s="102"/>
-      <c r="L21" s="102"/>
-      <c r="M21" s="103"/>
+      <c r="K21" s="94"/>
+      <c r="L21" s="94"/>
+      <c r="M21" s="95"/>
       <c r="N21" s="17"/>
       <c r="O21" s="39"/>
       <c r="P21" s="40"/>
@@ -2775,22 +2847,22 @@
       <c r="AA22" s="46"/>
     </row>
     <row r="23" spans="2:27" s="9" customFormat="1" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="97" t="s">
+      <c r="B23" s="96" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="98"/>
-      <c r="D23" s="98"/>
-      <c r="E23" s="99"/>
-      <c r="F23" s="100"/>
+      <c r="C23" s="97"/>
+      <c r="D23" s="97"/>
+      <c r="E23" s="98"/>
+      <c r="F23" s="99"/>
       <c r="G23" s="24"/>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
-      <c r="J23" s="97" t="s">
+      <c r="J23" s="96" t="s">
         <v>52</v>
       </c>
-      <c r="K23" s="98"/>
-      <c r="L23" s="98"/>
-      <c r="M23" s="99"/>
+      <c r="K23" s="97"/>
+      <c r="L23" s="97"/>
+      <c r="M23" s="98"/>
       <c r="N23" s="15"/>
       <c r="O23" s="27"/>
       <c r="P23" s="28"/>
@@ -2807,22 +2879,22 @@
       <c r="AA23" s="32"/>
     </row>
     <row r="24" spans="2:27" s="9" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="101" t="s">
+      <c r="B24" s="93" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="102"/>
-      <c r="D24" s="102"/>
-      <c r="E24" s="103"/>
-      <c r="F24" s="100"/>
+      <c r="C24" s="94"/>
+      <c r="D24" s="94"/>
+      <c r="E24" s="95"/>
+      <c r="F24" s="99"/>
       <c r="G24" s="26"/>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
-      <c r="J24" s="101" t="s">
+      <c r="J24" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="K24" s="102"/>
-      <c r="L24" s="102"/>
-      <c r="M24" s="103"/>
+      <c r="K24" s="94"/>
+      <c r="L24" s="94"/>
+      <c r="M24" s="95"/>
       <c r="N24" s="17"/>
       <c r="O24" s="39"/>
       <c r="P24" s="40"/>
@@ -2921,24 +2993,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="I2:AA3"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="B2:G3"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="J10:M10"/>
-    <mergeCell ref="J11:M11"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="J20:M20"/>
@@ -2955,6 +3009,24 @@
     <mergeCell ref="J17:M17"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B21:E21"/>
+    <mergeCell ref="I2:AA3"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="B2:G3"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="J10:M10"/>
+    <mergeCell ref="J11:M11"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="J24:M24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Pass data from API message to Trade object
Pass data from API message to Trade object and collecting data to write to the Excel file
</commit_message>
<xml_diff>
--- a/trading_journal.xlsx
+++ b/trading_journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Cloud Files\TradingTools\trade_journal_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E58C2E-A040-479A-9EED-0E47942485D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C6D386-DAD9-4C27-81EC-DBE06981F56A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
   <si>
     <t>Sector</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>lmt</t>
+  </si>
+  <si>
+    <t>limit/stop</t>
   </si>
 </sst>
 </file>
@@ -336,7 +339,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="32">
+  <fills count="31">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -491,31 +494,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1118,7 +1115,7 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1293,6 +1290,18 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1350,12 +1359,6 @@
     <xf numFmtId="0" fontId="5" fillId="25" borderId="25" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1365,8 +1368,17 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1377,17 +1389,14 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="16" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1411,15 +1420,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1437,37 +1437,37 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="16" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="9" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="28" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="30" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1779,7 +1779,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P20" sqref="P20"/>
+      <selection pane="bottomRight" activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" thickBottom="1" x14ac:dyDescent="0.35"/>
@@ -1815,44 +1815,44 @@
     <row r="1" spans="1:55" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="68"/>
-      <c r="W1" s="68"/>
-      <c r="X1" s="68"/>
-      <c r="Y1" s="68"/>
-      <c r="Z1" s="68"/>
-      <c r="AA1" s="68"/>
-      <c r="AB1" s="68"/>
-      <c r="AC1" s="68"/>
-      <c r="AD1" s="68"/>
-      <c r="AE1" s="68"/>
-      <c r="AF1" s="68"/>
-      <c r="AG1" s="68"/>
-      <c r="AH1" s="68"/>
-      <c r="AI1" s="68"/>
-      <c r="AJ1" s="68"/>
-      <c r="AK1" s="68"/>
-      <c r="AL1" s="68"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
+      <c r="P1" s="72"/>
+      <c r="Q1" s="72"/>
+      <c r="R1" s="72"/>
+      <c r="S1" s="72"/>
+      <c r="T1" s="72"/>
+      <c r="U1" s="72"/>
+      <c r="V1" s="72"/>
+      <c r="W1" s="72"/>
+      <c r="X1" s="72"/>
+      <c r="Y1" s="72"/>
+      <c r="Z1" s="72"/>
+      <c r="AA1" s="72"/>
+      <c r="AB1" s="72"/>
+      <c r="AC1" s="72"/>
+      <c r="AD1" s="72"/>
+      <c r="AE1" s="72"/>
+      <c r="AF1" s="72"/>
+      <c r="AG1" s="72"/>
+      <c r="AH1" s="72"/>
+      <c r="AI1" s="72"/>
+      <c r="AJ1" s="72"/>
+      <c r="AK1" s="72"/>
+      <c r="AL1" s="72"/>
       <c r="AM1" s="4"/>
       <c r="AN1" s="4"/>
       <c r="AO1" s="4"/>
@@ -1916,83 +1916,83 @@
       <c r="BC2" s="7"/>
     </row>
     <row r="3" spans="1:55" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="79" t="s">
+      <c r="C3" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="71" t="s">
+      <c r="D3" s="75" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="81" t="s">
+      <c r="E3" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="81" t="s">
+      <c r="F3" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="78" t="s">
+      <c r="G3" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78" t="s">
+      <c r="H3" s="82"/>
+      <c r="I3" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="78"/>
-      <c r="K3" s="89" t="s">
+      <c r="J3" s="82"/>
+      <c r="K3" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="90"/>
-      <c r="M3" s="90"/>
-      <c r="N3" s="90"/>
-      <c r="O3" s="90"/>
-      <c r="P3" s="90"/>
-      <c r="Q3" s="91"/>
-      <c r="R3" s="75" t="s">
+      <c r="L3" s="92"/>
+      <c r="M3" s="92"/>
+      <c r="N3" s="92"/>
+      <c r="O3" s="92"/>
+      <c r="P3" s="92"/>
+      <c r="Q3" s="93"/>
+      <c r="R3" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="75"/>
-      <c r="T3" s="75"/>
-      <c r="U3" s="75"/>
-      <c r="V3" s="92" t="s">
+      <c r="S3" s="79"/>
+      <c r="T3" s="79"/>
+      <c r="U3" s="79"/>
+      <c r="V3" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="W3" s="92"/>
-      <c r="X3" s="92"/>
-      <c r="Y3" s="73" t="s">
+      <c r="W3" s="69"/>
+      <c r="X3" s="69"/>
+      <c r="Y3" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="Z3" s="73" t="s">
+      <c r="Z3" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="AA3" s="86" t="s">
+      <c r="AA3" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="AB3" s="86"/>
-      <c r="AC3" s="83" t="s">
+      <c r="AB3" s="90"/>
+      <c r="AC3" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="AD3" s="84"/>
-      <c r="AE3" s="84"/>
-      <c r="AF3" s="84"/>
-      <c r="AG3" s="84"/>
-      <c r="AH3" s="85"/>
-      <c r="AI3" s="87" t="s">
+      <c r="AD3" s="88"/>
+      <c r="AE3" s="88"/>
+      <c r="AF3" s="88"/>
+      <c r="AG3" s="88"/>
+      <c r="AH3" s="89"/>
+      <c r="AI3" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="AJ3" s="87" t="s">
+      <c r="AJ3" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="AK3" s="69" t="s">
+      <c r="AK3" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="AL3" s="76" t="s">
+      <c r="AL3" s="80" t="s">
         <v>19</v>
       </c>
       <c r="AP3" s="6"/>
     </row>
     <row r="4" spans="1:55" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="80"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
       <c r="G4" s="63" t="s">
         <v>4</v>
       </c>
@@ -2047,8 +2047,8 @@
       <c r="X4" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="Y4" s="74"/>
-      <c r="Z4" s="74"/>
+      <c r="Y4" s="78"/>
+      <c r="Z4" s="78"/>
       <c r="AA4" s="62" t="s">
         <v>4</v>
       </c>
@@ -2073,38 +2073,40 @@
       <c r="AH4" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="AI4" s="88"/>
-      <c r="AJ4" s="88"/>
-      <c r="AK4" s="70"/>
-      <c r="AL4" s="77"/>
+      <c r="AI4" s="71"/>
+      <c r="AJ4" s="71"/>
+      <c r="AK4" s="74"/>
+      <c r="AL4" s="81"/>
     </row>
     <row r="5" spans="1:55" ht="14.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="118"/>
-      <c r="D5" s="116"/>
-      <c r="E5" s="119"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="117"/>
       <c r="F5" s="117"/>
-      <c r="G5" s="120"/>
-      <c r="H5" s="120"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
+      <c r="G5" s="117"/>
+      <c r="H5" s="117"/>
+      <c r="I5" s="125"/>
+      <c r="J5" s="125"/>
       <c r="K5" s="117"/>
       <c r="L5" s="117"/>
-      <c r="M5" s="120"/>
-      <c r="N5" s="117" t="s">
+      <c r="M5" s="117" t="s">
+        <v>67</v>
+      </c>
+      <c r="N5" s="125" t="s">
         <v>66</v>
       </c>
       <c r="O5" s="117"/>
-      <c r="P5" s="48"/>
-      <c r="Q5" s="48"/>
+      <c r="P5" s="125"/>
+      <c r="Q5" s="125"/>
       <c r="R5" s="48"/>
-      <c r="S5" s="48"/>
-      <c r="T5" s="48"/>
-      <c r="U5" s="48"/>
+      <c r="S5" s="68"/>
+      <c r="T5" s="125"/>
+      <c r="U5" s="125"/>
       <c r="V5" s="117"/>
-      <c r="W5" s="120"/>
-      <c r="X5" s="120"/>
-      <c r="Y5" s="48"/>
-      <c r="Z5" s="122"/>
+      <c r="W5" s="125"/>
+      <c r="X5" s="125"/>
+      <c r="Y5" s="125"/>
+      <c r="Z5" s="68"/>
       <c r="AA5" s="48"/>
       <c r="AB5" s="48"/>
       <c r="AC5" s="48"/>
@@ -2113,15 +2115,21 @@
       <c r="AF5" s="48"/>
       <c r="AG5" s="48"/>
       <c r="AH5" s="48"/>
-      <c r="AI5" s="123"/>
-      <c r="AJ5" s="124"/>
-      <c r="AK5" s="125"/>
-      <c r="AL5" s="126"/>
+      <c r="AI5" s="119"/>
+      <c r="AJ5" s="120"/>
+      <c r="AK5" s="121"/>
+      <c r="AL5" s="122"/>
     </row>
     <row r="6" spans="1:55" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="N6" s="121" t="s">
+      <c r="M6" s="127" t="s">
         <v>65</v>
       </c>
+      <c r="N6" s="126" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:55" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G7" s="123"/>
     </row>
     <row r="26" spans="34:35" thickBot="1" x14ac:dyDescent="0.35">
       <c r="AH26" s="51"/>
@@ -2129,6 +2137,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="AJ3:AJ4"/>
+    <mergeCell ref="K3:Q3"/>
     <mergeCell ref="V3:X3"/>
     <mergeCell ref="AI3:AI4"/>
     <mergeCell ref="C1:AL1"/>
@@ -2145,8 +2155,6 @@
     <mergeCell ref="Z3:Z4"/>
     <mergeCell ref="AC3:AH3"/>
     <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AJ3:AJ4"/>
-    <mergeCell ref="K3:Q3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2183,64 +2191,64 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="100" t="s">
+      <c r="B2" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
       <c r="H2" s="23"/>
-      <c r="I2" s="100" t="s">
+      <c r="I2" s="104" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="100"/>
-      <c r="M2" s="100"/>
-      <c r="N2" s="100"/>
-      <c r="O2" s="100"/>
-      <c r="P2" s="100"/>
-      <c r="Q2" s="100"/>
-      <c r="R2" s="100"/>
-      <c r="S2" s="100"/>
-      <c r="T2" s="100"/>
-      <c r="U2" s="100"/>
-      <c r="V2" s="100"/>
-      <c r="W2" s="100"/>
-      <c r="X2" s="100"/>
-      <c r="Y2" s="100"/>
-      <c r="Z2" s="100"/>
-      <c r="AA2" s="100"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104"/>
+      <c r="M2" s="104"/>
+      <c r="N2" s="104"/>
+      <c r="O2" s="104"/>
+      <c r="P2" s="104"/>
+      <c r="Q2" s="104"/>
+      <c r="R2" s="104"/>
+      <c r="S2" s="104"/>
+      <c r="T2" s="104"/>
+      <c r="U2" s="104"/>
+      <c r="V2" s="104"/>
+      <c r="W2" s="104"/>
+      <c r="X2" s="104"/>
+      <c r="Y2" s="104"/>
+      <c r="Z2" s="104"/>
+      <c r="AA2" s="104"/>
     </row>
     <row r="3" spans="1:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
+      <c r="B3" s="104"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
       <c r="H3" s="23"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="100"/>
-      <c r="K3" s="100"/>
-      <c r="L3" s="100"/>
-      <c r="M3" s="100"/>
-      <c r="N3" s="100"/>
-      <c r="O3" s="100"/>
-      <c r="P3" s="100"/>
-      <c r="Q3" s="100"/>
-      <c r="R3" s="100"/>
-      <c r="S3" s="100"/>
-      <c r="T3" s="100"/>
-      <c r="U3" s="100"/>
-      <c r="V3" s="100"/>
-      <c r="W3" s="100"/>
-      <c r="X3" s="100"/>
-      <c r="Y3" s="100"/>
-      <c r="Z3" s="100"/>
-      <c r="AA3" s="100"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="104"/>
+      <c r="L3" s="104"/>
+      <c r="M3" s="104"/>
+      <c r="N3" s="104"/>
+      <c r="O3" s="104"/>
+      <c r="P3" s="104"/>
+      <c r="Q3" s="104"/>
+      <c r="R3" s="104"/>
+      <c r="S3" s="104"/>
+      <c r="T3" s="104"/>
+      <c r="U3" s="104"/>
+      <c r="V3" s="104"/>
+      <c r="W3" s="104"/>
+      <c r="X3" s="104"/>
+      <c r="Y3" s="104"/>
+      <c r="Z3" s="104"/>
+      <c r="AA3" s="104"/>
     </row>
     <row r="4" spans="1:27" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="10"/>
@@ -2277,11 +2285,11 @@
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
-      <c r="J5" s="104" t="s">
+      <c r="J5" s="108" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="105"/>
-      <c r="L5" s="106"/>
+      <c r="K5" s="109"/>
+      <c r="L5" s="110"/>
       <c r="M5" s="14"/>
       <c r="N5" s="12"/>
       <c r="O5" s="52" t="s">
@@ -2353,21 +2361,21 @@
       <c r="AA6" s="20"/>
     </row>
     <row r="7" spans="1:27" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="96" t="s">
+      <c r="B7" s="94" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="97"/>
-      <c r="D7" s="97"/>
-      <c r="E7" s="98"/>
-      <c r="F7" s="99"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="95"/>
+      <c r="E7" s="96"/>
+      <c r="F7" s="97"/>
       <c r="G7" s="24"/>
       <c r="I7" s="10"/>
-      <c r="J7" s="101" t="s">
+      <c r="J7" s="105" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="102"/>
-      <c r="L7" s="102"/>
-      <c r="M7" s="103"/>
+      <c r="K7" s="106"/>
+      <c r="L7" s="106"/>
+      <c r="M7" s="107"/>
       <c r="N7" s="15"/>
       <c r="O7" s="27"/>
       <c r="P7" s="28"/>
@@ -2384,13 +2392,13 @@
       <c r="AA7" s="32"/>
     </row>
     <row r="8" spans="1:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="107" t="s">
+      <c r="B8" s="101" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="108"/>
-      <c r="D8" s="108"/>
-      <c r="E8" s="109"/>
-      <c r="F8" s="99"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="102"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="97"/>
       <c r="G8" s="25"/>
       <c r="I8" s="10"/>
       <c r="J8" s="57" t="s">
@@ -2415,13 +2423,13 @@
       <c r="AA8" s="38"/>
     </row>
     <row r="9" spans="1:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="107" t="s">
+      <c r="B9" s="101" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="108"/>
-      <c r="D9" s="108"/>
-      <c r="E9" s="109"/>
-      <c r="F9" s="99"/>
+      <c r="C9" s="102"/>
+      <c r="D9" s="102"/>
+      <c r="E9" s="103"/>
+      <c r="F9" s="97"/>
       <c r="G9" s="25"/>
       <c r="I9" s="10"/>
       <c r="J9" s="57" t="s">
@@ -2446,21 +2454,21 @@
       <c r="AA9" s="38"/>
     </row>
     <row r="10" spans="1:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="107" t="s">
+      <c r="B10" s="101" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="108"/>
-      <c r="D10" s="108"/>
-      <c r="E10" s="109"/>
-      <c r="F10" s="99"/>
+      <c r="C10" s="102"/>
+      <c r="D10" s="102"/>
+      <c r="E10" s="103"/>
+      <c r="F10" s="97"/>
       <c r="G10" s="25"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="110" t="s">
+      <c r="J10" s="111" t="s">
         <v>28</v>
       </c>
-      <c r="K10" s="111"/>
-      <c r="L10" s="111"/>
-      <c r="M10" s="112"/>
+      <c r="K10" s="112"/>
+      <c r="L10" s="112"/>
+      <c r="M10" s="113"/>
       <c r="N10" s="17"/>
       <c r="O10" s="33"/>
       <c r="P10" s="34"/>
@@ -2477,21 +2485,21 @@
       <c r="AA10" s="38"/>
     </row>
     <row r="11" spans="1:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="93" t="s">
+      <c r="B11" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="94"/>
-      <c r="D11" s="94"/>
-      <c r="E11" s="95"/>
-      <c r="F11" s="99"/>
+      <c r="C11" s="99"/>
+      <c r="D11" s="99"/>
+      <c r="E11" s="100"/>
+      <c r="F11" s="97"/>
       <c r="G11" s="26"/>
       <c r="I11" s="10"/>
-      <c r="J11" s="113" t="s">
+      <c r="J11" s="114" t="s">
         <v>29</v>
       </c>
-      <c r="K11" s="114"/>
-      <c r="L11" s="114"/>
-      <c r="M11" s="115"/>
+      <c r="K11" s="115"/>
+      <c r="L11" s="115"/>
+      <c r="M11" s="116"/>
       <c r="N11" s="21"/>
       <c r="O11" s="39"/>
       <c r="P11" s="40"/>
@@ -2537,22 +2545,22 @@
     </row>
     <row r="13" spans="1:27" s="7" customFormat="1" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
-      <c r="B13" s="96" t="s">
+      <c r="B13" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="97"/>
-      <c r="D13" s="97"/>
-      <c r="E13" s="98"/>
-      <c r="F13" s="99"/>
+      <c r="C13" s="95"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="96"/>
+      <c r="F13" s="97"/>
       <c r="G13" s="24"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
-      <c r="J13" s="96" t="s">
+      <c r="J13" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="K13" s="97"/>
-      <c r="L13" s="97"/>
-      <c r="M13" s="98"/>
+      <c r="K13" s="95"/>
+      <c r="L13" s="95"/>
+      <c r="M13" s="96"/>
       <c r="N13" s="22"/>
       <c r="O13" s="27"/>
       <c r="P13" s="28"/>
@@ -2570,22 +2578,22 @@
     </row>
     <row r="14" spans="1:27" s="7" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
-      <c r="B14" s="107" t="s">
+      <c r="B14" s="101" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="108"/>
-      <c r="D14" s="108"/>
-      <c r="E14" s="109"/>
-      <c r="F14" s="99"/>
+      <c r="C14" s="102"/>
+      <c r="D14" s="102"/>
+      <c r="E14" s="103"/>
+      <c r="F14" s="97"/>
       <c r="G14" s="25"/>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
-      <c r="J14" s="107" t="s">
+      <c r="J14" s="101" t="s">
         <v>31</v>
       </c>
-      <c r="K14" s="108"/>
-      <c r="L14" s="108"/>
-      <c r="M14" s="109"/>
+      <c r="K14" s="102"/>
+      <c r="L14" s="102"/>
+      <c r="M14" s="103"/>
       <c r="N14" s="22"/>
       <c r="O14" s="33"/>
       <c r="P14" s="34"/>
@@ -2603,22 +2611,22 @@
     </row>
     <row r="15" spans="1:27" s="7" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
-      <c r="B15" s="93" t="s">
+      <c r="B15" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="94"/>
-      <c r="D15" s="94"/>
-      <c r="E15" s="95"/>
-      <c r="F15" s="99"/>
+      <c r="C15" s="99"/>
+      <c r="D15" s="99"/>
+      <c r="E15" s="100"/>
+      <c r="F15" s="97"/>
       <c r="G15" s="26"/>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
-      <c r="J15" s="93" t="s">
+      <c r="J15" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="K15" s="94"/>
-      <c r="L15" s="94"/>
-      <c r="M15" s="95"/>
+      <c r="K15" s="99"/>
+      <c r="L15" s="99"/>
+      <c r="M15" s="100"/>
       <c r="N15" s="22"/>
       <c r="O15" s="39"/>
       <c r="P15" s="40"/>
@@ -2663,22 +2671,22 @@
       <c r="AA16" s="46"/>
     </row>
     <row r="17" spans="2:27" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="96" t="s">
+      <c r="B17" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="97"/>
-      <c r="D17" s="97"/>
-      <c r="E17" s="98"/>
-      <c r="F17" s="99"/>
+      <c r="C17" s="95"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="96"/>
+      <c r="F17" s="97"/>
       <c r="G17" s="24"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="96" t="s">
+      <c r="J17" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="K17" s="97"/>
-      <c r="L17" s="97"/>
-      <c r="M17" s="98"/>
+      <c r="K17" s="95"/>
+      <c r="L17" s="95"/>
+      <c r="M17" s="96"/>
       <c r="N17" s="15"/>
       <c r="O17" s="27"/>
       <c r="P17" s="28"/>
@@ -2695,22 +2703,22 @@
       <c r="AA17" s="32"/>
     </row>
     <row r="18" spans="2:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="93" t="s">
+      <c r="B18" s="98" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="94"/>
-      <c r="D18" s="94"/>
-      <c r="E18" s="95"/>
-      <c r="F18" s="99"/>
+      <c r="C18" s="99"/>
+      <c r="D18" s="99"/>
+      <c r="E18" s="100"/>
+      <c r="F18" s="97"/>
       <c r="G18" s="26"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
-      <c r="J18" s="93" t="s">
+      <c r="J18" s="98" t="s">
         <v>34</v>
       </c>
-      <c r="K18" s="94"/>
-      <c r="L18" s="94"/>
-      <c r="M18" s="95"/>
+      <c r="K18" s="99"/>
+      <c r="L18" s="99"/>
+      <c r="M18" s="100"/>
       <c r="N18" s="17"/>
       <c r="O18" s="39"/>
       <c r="P18" s="40"/>
@@ -2755,22 +2763,22 @@
       <c r="AA19" s="46"/>
     </row>
     <row r="20" spans="2:27" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="96" t="s">
+      <c r="B20" s="94" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="97"/>
-      <c r="D20" s="97"/>
-      <c r="E20" s="98"/>
-      <c r="F20" s="99"/>
+      <c r="C20" s="95"/>
+      <c r="D20" s="95"/>
+      <c r="E20" s="96"/>
+      <c r="F20" s="97"/>
       <c r="G20" s="24"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
-      <c r="J20" s="96" t="s">
+      <c r="J20" s="94" t="s">
         <v>52</v>
       </c>
-      <c r="K20" s="97"/>
-      <c r="L20" s="97"/>
-      <c r="M20" s="98"/>
+      <c r="K20" s="95"/>
+      <c r="L20" s="95"/>
+      <c r="M20" s="96"/>
       <c r="N20" s="15"/>
       <c r="O20" s="27"/>
       <c r="P20" s="28"/>
@@ -2787,22 +2795,22 @@
       <c r="AA20" s="32"/>
     </row>
     <row r="21" spans="2:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="93" t="s">
+      <c r="B21" s="98" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="94"/>
-      <c r="D21" s="94"/>
-      <c r="E21" s="95"/>
-      <c r="F21" s="99"/>
+      <c r="C21" s="99"/>
+      <c r="D21" s="99"/>
+      <c r="E21" s="100"/>
+      <c r="F21" s="97"/>
       <c r="G21" s="26"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="93" t="s">
+      <c r="J21" s="98" t="s">
         <v>53</v>
       </c>
-      <c r="K21" s="94"/>
-      <c r="L21" s="94"/>
-      <c r="M21" s="95"/>
+      <c r="K21" s="99"/>
+      <c r="L21" s="99"/>
+      <c r="M21" s="100"/>
       <c r="N21" s="17"/>
       <c r="O21" s="39"/>
       <c r="P21" s="40"/>
@@ -2847,22 +2855,22 @@
       <c r="AA22" s="46"/>
     </row>
     <row r="23" spans="2:27" s="9" customFormat="1" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="96" t="s">
+      <c r="B23" s="94" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="97"/>
-      <c r="D23" s="97"/>
-      <c r="E23" s="98"/>
-      <c r="F23" s="99"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="96"/>
+      <c r="F23" s="97"/>
       <c r="G23" s="24"/>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
-      <c r="J23" s="96" t="s">
+      <c r="J23" s="94" t="s">
         <v>52</v>
       </c>
-      <c r="K23" s="97"/>
-      <c r="L23" s="97"/>
-      <c r="M23" s="98"/>
+      <c r="K23" s="95"/>
+      <c r="L23" s="95"/>
+      <c r="M23" s="96"/>
       <c r="N23" s="15"/>
       <c r="O23" s="27"/>
       <c r="P23" s="28"/>
@@ -2879,22 +2887,22 @@
       <c r="AA23" s="32"/>
     </row>
     <row r="24" spans="2:27" s="9" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="93" t="s">
+      <c r="B24" s="98" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="94"/>
-      <c r="D24" s="94"/>
-      <c r="E24" s="95"/>
-      <c r="F24" s="99"/>
+      <c r="C24" s="99"/>
+      <c r="D24" s="99"/>
+      <c r="E24" s="100"/>
+      <c r="F24" s="97"/>
       <c r="G24" s="26"/>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
-      <c r="J24" s="93" t="s">
+      <c r="J24" s="98" t="s">
         <v>53</v>
       </c>
-      <c r="K24" s="94"/>
-      <c r="L24" s="94"/>
-      <c r="M24" s="95"/>
+      <c r="K24" s="99"/>
+      <c r="L24" s="99"/>
+      <c r="M24" s="100"/>
       <c r="N24" s="17"/>
       <c r="O24" s="39"/>
       <c r="P24" s="40"/>
@@ -2993,6 +3001,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="J24:M24"/>
+    <mergeCell ref="I2:AA3"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="B2:G3"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="J10:M10"/>
+    <mergeCell ref="J11:M11"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="J20:M20"/>
@@ -3009,24 +3035,6 @@
     <mergeCell ref="J17:M17"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B21:E21"/>
-    <mergeCell ref="I2:AA3"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="B2:G3"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="J10:M10"/>
-    <mergeCell ref="J11:M11"/>
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="J24:M24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>